<commit_message>
v10: Majore release - New Motor control algorithm: 	- IRQ based Hall detection 	- Hall counter @ 250KHz 	- Hall Calibration (Angular and Time correction) 	- Hall counter correction based on Hall state 	- Phase adjust step by step - HW tirggered ADC conversion (OC4Ref) - Added calibration mode to riding modes
</commit_message>
<xml_diff>
--- a/PWMCalculations.xlsx
+++ b/PWMCalculations.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Massimo\Priv\Ebk\TSDZ2\BT\TSDZ2_ESP32\TSDZ2-Smart-EBike-Dev\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Massimo\Priv\Ebk\TSDZ2\BT\TSDZ2_ESP32\TSDZ2-Smart-EBike\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{725C9FED-1909-4FF8-BF9C-62850A037C1B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D69F28-7A20-4344-9CCC-B1D1972DF03C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4608" yWindow="396" windowWidth="18144" windowHeight="12240" xr2:uid="{0FECAB06-F1EB-47DE-95C0-CE04C98C7007}"/>
+    <workbookView xWindow="24" yWindow="0" windowWidth="21276" windowHeight="12240" activeTab="1" xr2:uid="{0FECAB06-F1EB-47DE-95C0-CE04C98C7007}"/>
   </bookViews>
   <sheets>
     <sheet name="Ref. Values" sheetId="1" r:id="rId1"/>
@@ -214,10 +214,10 @@
     <t>New SW has an offset angle of 4 (roundx256)  and adds an average offset of 33 counter step to only turn/6 counter</t>
   </si>
   <si>
-    <t>The offset added to the Hall counter is 23 for the states whit a falling edge of the Hall value and 43 to the state with a rising edge (avg = 33)</t>
+    <t>Field Weakening offset max</t>
   </si>
   <si>
-    <t>Field Weakening offset max</t>
+    <t>The offset added to the Hall counter is 23 for the states whit a falling edge of the Hall value and 44 to the state with a rising edge (avg = 33,5)</t>
   </si>
 </sst>
 </file>
@@ -2072,7 +2072,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="130"/>
                 <c:pt idx="0">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>21</c:v>
@@ -2090,10 +2090,10 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>20</c:v>
@@ -2114,10 +2114,10 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="16">
                   <c:v>19</c:v>
@@ -2135,10 +2135,10 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>18</c:v>
@@ -2156,10 +2156,10 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>17</c:v>
@@ -2180,7 +2180,7 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="37">
                   <c:v>16</c:v>
@@ -2201,10 +2201,10 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>15</c:v>
@@ -2222,10 +2222,10 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>14</c:v>
@@ -2246,7 +2246,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="59">
                   <c:v>13</c:v>
@@ -2267,7 +2267,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>12</c:v>
@@ -2291,7 +2291,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="74">
                   <c:v>11</c:v>
@@ -2312,7 +2312,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="81">
                   <c:v>10</c:v>
@@ -2333,7 +2333,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="88">
                   <c:v>9</c:v>
@@ -2378,7 +2378,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="103">
                   <c:v>7</c:v>
@@ -2399,7 +2399,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="110">
                   <c:v>6</c:v>
@@ -2928,10 +2928,10 @@
                   <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>25</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>24</c:v>
@@ -2946,10 +2946,10 @@
                   <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>23</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="11">
                   <c:v>23</c:v>
@@ -2967,7 +2967,7 @@
                   <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>22</c:v>
+                  <c:v>23</c:v>
                 </c:pt>
                 <c:pt idx="17">
                   <c:v>22</c:v>
@@ -2985,7 +2985,7 @@
                   <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>21</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>21</c:v>
@@ -3003,10 +3003,10 @@
                   <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>20</c:v>
+                  <c:v>21</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>20</c:v>
@@ -3021,10 +3021,10 @@
                   <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>19</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="36">
                   <c:v>19</c:v>
@@ -3039,10 +3039,10 @@
                   <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>18</c:v>
+                  <c:v>19</c:v>
                 </c:pt>
                 <c:pt idx="42">
                   <c:v>18</c:v>
@@ -3057,10 +3057,10 @@
                   <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>17</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="48">
                   <c:v>17</c:v>
@@ -3078,7 +3078,7 @@
                   <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>16</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="54">
                   <c:v>16</c:v>
@@ -3096,7 +3096,7 @@
                   <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>15</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="60">
                   <c:v>15</c:v>
@@ -3114,7 +3114,7 @@
                   <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>14</c:v>
+                  <c:v>15</c:v>
                 </c:pt>
                 <c:pt idx="66">
                   <c:v>14</c:v>
@@ -3132,7 +3132,7 @@
                   <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>13</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="72">
                   <c:v>13</c:v>
@@ -3150,7 +3150,7 @@
                   <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>12</c:v>
+                  <c:v>13</c:v>
                 </c:pt>
                 <c:pt idx="78">
                   <c:v>12</c:v>
@@ -3168,7 +3168,7 @@
                   <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="84">
                   <c:v>11</c:v>
@@ -3186,7 +3186,7 @@
                   <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>10</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="90">
                   <c:v>10</c:v>
@@ -3204,7 +3204,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>9</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="96">
                   <c:v>9</c:v>
@@ -3222,7 +3222,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>8</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="102">
                   <c:v>8</c:v>
@@ -3240,7 +3240,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>7</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="108">
                   <c:v>7</c:v>
@@ -3258,7 +3258,7 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>6</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="114">
                   <c:v>6</c:v>
@@ -3276,7 +3276,7 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>5</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="120">
                   <c:v>5</c:v>
@@ -3294,7 +3294,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>4</c:v>
+                  <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="126">
                   <c:v>4</c:v>
@@ -4418,7 +4418,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{652CF362-57A8-41E9-B80F-B52BC9767EEC}">
   <dimension ref="A1:L51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="C18" sqref="C18:H18"/>
     </sheetView>
   </sheetViews>
@@ -5548,8 +5548,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA1CD390-437C-4C87-9147-4AC4215597A8}">
   <dimension ref="A1:U141"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5574,12 +5574,12 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="26" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="D5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G5">
         <v>6</v>
@@ -5604,7 +5604,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="38">
-        <v>33</v>
+        <v>33.5</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -5670,7 +5670,7 @@
       </c>
       <c r="F11" s="28">
         <f>TRUNC((($F$7-$F$8)*256)/C11)+F$6</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G11" s="36">
         <f>TRUNC((($F$7-$F$8+$G$5)*256)/(C11+F$8))+F$6</f>
@@ -5699,7 +5699,7 @@
       </c>
       <c r="F12" s="28">
         <f t="shared" ref="F12:F75" si="4">TRUNC((($F$7-$F$8)*256)/C12)+F$6</f>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G12" s="36">
         <f t="shared" ref="G12:G75" si="5">TRUNC((($F$7-$F$8+$G$5)*256)/(C12+F$8))+F$6</f>
@@ -5794,7 +5794,7 @@
       </c>
       <c r="G15" s="36">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.3">
@@ -5823,7 +5823,7 @@
       </c>
       <c r="G16" s="36">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
@@ -5877,7 +5877,7 @@
       </c>
       <c r="F18" s="28">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G18" s="36">
         <f t="shared" si="5"/>
@@ -5906,7 +5906,7 @@
       </c>
       <c r="F19" s="28">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G19" s="36">
         <f t="shared" si="5"/>
@@ -5968,7 +5968,7 @@
       </c>
       <c r="G21" s="36">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
@@ -5997,7 +5997,7 @@
       </c>
       <c r="G22" s="36">
         <f t="shared" si="5"/>
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
@@ -6109,7 +6109,7 @@
       </c>
       <c r="F26" s="28">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G26" s="36">
         <f t="shared" si="5"/>
@@ -6138,7 +6138,7 @@
       </c>
       <c r="F27" s="28">
         <f t="shared" si="4"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="G27" s="36">
         <f t="shared" si="5"/>
@@ -6171,7 +6171,7 @@
       </c>
       <c r="G28" s="36">
         <f t="shared" si="5"/>
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
@@ -6312,7 +6312,7 @@
       </c>
       <c r="F33" s="28">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G33" s="36">
         <f t="shared" si="5"/>
@@ -6341,11 +6341,11 @@
       </c>
       <c r="F34" s="28">
         <f t="shared" si="4"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G34" s="36">
         <f t="shared" si="5"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H34" t="s">
         <v>18</v>
@@ -6585,11 +6585,11 @@
       </c>
       <c r="F40" s="28">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G40" s="36">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H40" s="57"/>
       <c r="I40" s="58"/>
@@ -6627,11 +6627,11 @@
       </c>
       <c r="F41" s="28">
         <f t="shared" si="4"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="G41" s="36">
         <f t="shared" si="5"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="H41" s="57"/>
       <c r="I41" s="58"/>
@@ -6841,7 +6841,7 @@
       </c>
       <c r="G46" s="36">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="H46" s="57"/>
       <c r="I46" s="58"/>
@@ -6882,7 +6882,7 @@
       </c>
       <c r="G47" s="36">
         <f t="shared" si="5"/>
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="48" spans="1:20" x14ac:dyDescent="0.3">
@@ -6907,18 +6907,14 @@
       </c>
       <c r="F48" s="28">
         <f t="shared" si="4"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G48" s="36">
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="I48">
-        <f>256*533.3/250000</f>
-        <v>0.54609920000000001</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="26">
         <f t="shared" si="0"/>
         <v>85.14492753623189</v>
@@ -6946,16 +6942,8 @@
         <f t="shared" si="5"/>
         <v>19</v>
       </c>
-      <c r="I49">
-        <f>1/I48</f>
-        <v>1.8311691355709732</v>
-      </c>
-      <c r="J49">
-        <f>I49*4</f>
-        <v>7.3246765422838926</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="26">
         <f t="shared" si="0"/>
         <v>84.239130434782624</v>
@@ -6984,7 +6972,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="26">
         <f t="shared" si="0"/>
         <v>83.333333333333329</v>
@@ -7013,7 +7001,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="26">
         <f t="shared" si="0"/>
         <v>82.427536231884062</v>
@@ -7039,10 +7027,10 @@
       </c>
       <c r="G52" s="36">
         <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="26">
         <f t="shared" si="0"/>
         <v>81.521739130434781</v>
@@ -7068,10 +7056,10 @@
       </c>
       <c r="G53" s="36">
         <f t="shared" si="5"/>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="26">
         <f t="shared" si="0"/>
         <v>80.615942028985515</v>
@@ -7100,7 +7088,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="26">
         <f t="shared" si="0"/>
         <v>79.710144927536234</v>
@@ -7122,14 +7110,14 @@
       </c>
       <c r="F55" s="28">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G55" s="36">
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
     </row>
-    <row r="56" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="26">
         <f t="shared" si="0"/>
         <v>78.804347826086953</v>
@@ -7151,14 +7139,14 @@
       </c>
       <c r="F56" s="28">
         <f t="shared" si="4"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G56" s="36">
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
     </row>
-    <row r="57" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="26">
         <f t="shared" si="0"/>
         <v>77.898550724637687</v>
@@ -7187,7 +7175,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="58" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="26">
         <f t="shared" si="0"/>
         <v>76.992753623188406</v>
@@ -7213,10 +7201,10 @@
       </c>
       <c r="G58" s="36">
         <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="26">
         <f t="shared" si="0"/>
         <v>76.08695652173914</v>
@@ -7242,10 +7230,10 @@
       </c>
       <c r="G59" s="36">
         <f t="shared" si="5"/>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="26">
         <f t="shared" si="0"/>
         <v>75.181159420289859</v>
@@ -7274,7 +7262,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="26">
         <f t="shared" si="0"/>
         <v>74.275362318840578</v>
@@ -7303,7 +7291,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="26">
         <f t="shared" si="0"/>
         <v>73.369565217391298</v>
@@ -7325,14 +7313,14 @@
       </c>
       <c r="F62" s="28">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G62" s="36">
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="26">
         <f t="shared" si="0"/>
         <v>72.463768115942031</v>
@@ -7354,14 +7342,14 @@
       </c>
       <c r="F63" s="28">
         <f t="shared" si="4"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G63" s="36">
         <f t="shared" si="5"/>
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="26">
         <f t="shared" si="0"/>
         <v>71.557971014492765</v>
@@ -7416,7 +7404,7 @@
       </c>
       <c r="G65" s="36">
         <f t="shared" si="5"/>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
@@ -7557,7 +7545,7 @@
       </c>
       <c r="F70" s="28">
         <f t="shared" si="4"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="G70" s="36">
         <f t="shared" si="5"/>
@@ -7590,7 +7578,7 @@
       </c>
       <c r="G71" s="36">
         <f t="shared" si="5"/>
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
@@ -7760,11 +7748,11 @@
       </c>
       <c r="F77" s="28">
         <f t="shared" si="10"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="G77" s="36">
         <f t="shared" si="11"/>
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.3">
@@ -7938,7 +7926,7 @@
       </c>
       <c r="G83" s="36">
         <f t="shared" si="11"/>
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.3">
@@ -7992,7 +7980,7 @@
       </c>
       <c r="F85" s="28">
         <f t="shared" si="10"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G85" s="36">
         <f t="shared" si="11"/>
@@ -8112,7 +8100,7 @@
       </c>
       <c r="G89" s="36">
         <f t="shared" si="11"/>
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.3">
@@ -8195,7 +8183,7 @@
       </c>
       <c r="F92" s="28">
         <f t="shared" si="10"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G92" s="36">
         <f t="shared" si="11"/>
@@ -8286,7 +8274,7 @@
       </c>
       <c r="G95" s="36">
         <f t="shared" si="11"/>
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.3">
@@ -8398,7 +8386,7 @@
       </c>
       <c r="F99" s="28">
         <f t="shared" si="10"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="G99" s="36">
         <f t="shared" si="11"/>
@@ -8460,7 +8448,7 @@
       </c>
       <c r="G101" s="36">
         <f t="shared" si="11"/>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.3">
@@ -8634,7 +8622,7 @@
       </c>
       <c r="G107" s="36">
         <f t="shared" si="11"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.3">
@@ -8808,7 +8796,7 @@
       </c>
       <c r="G113" s="36">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.3">
@@ -8833,7 +8821,7 @@
       </c>
       <c r="F114" s="28">
         <f t="shared" si="10"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="G114" s="36">
         <f t="shared" si="11"/>
@@ -8982,7 +8970,7 @@
       </c>
       <c r="G119" s="36">
         <f t="shared" si="11"/>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.3">
@@ -9036,7 +9024,7 @@
       </c>
       <c r="F121" s="28">
         <f t="shared" si="10"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="G121" s="36">
         <f t="shared" si="11"/>
@@ -9156,7 +9144,7 @@
       </c>
       <c r="G125" s="36">
         <f t="shared" si="11"/>
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.3">
@@ -9330,7 +9318,7 @@
       </c>
       <c r="G131" s="36">
         <f t="shared" si="11"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.3">
@@ -9504,7 +9492,7 @@
       </c>
       <c r="G137" s="36">
         <f t="shared" si="11"/>
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>